<commit_message>
add README.md for preprocessing of data for NA screening analysis
</commit_message>
<xml_diff>
--- a/data/preprocessed/na_screening/cw_T1_preprocessed.xlsx
+++ b/data/preprocessed/na_screening/cw_T1_preprocessed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\preprocessed\na_screening\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32537135-23E5-4200-83E8-01949C0CBCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B35F3-56AA-48A1-9363-E520A5D8A654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,13 +220,13 @@
     <t>obs_well</t>
   </si>
   <si>
-    <t>pm_-xylene</t>
-  </si>
-  <si>
     <t>sulfate</t>
   </si>
   <si>
     <t>ug/l</t>
+  </si>
+  <si>
+    <t>pm_xylene</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +626,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -656,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>15</v>
@@ -676,31 +676,31 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
         <v>18</v>

</xml_diff>